<commit_message>
se guarda en hubspot location y move
</commit_message>
<xml_diff>
--- a/abstraccion-links.xlsx
+++ b/abstraccion-links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52a31a511a7e1632/Documents/PokeApi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PokeApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{0568697B-90D0-4342-8AF1-F02CD538A44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C70AD11-2785-4EF1-9E89-75EDA2571CB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2B077-4866-4D83-AE6B-EF1DDC018075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{134ECA9C-E322-42DE-933E-38BD1AE6EC15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="83">
   <si>
     <t>Pokémon property</t>
   </si>
@@ -285,12 +285,45 @@
   <si>
     <t>url: "https://pokeapi.co/api/v2/move/29/"</t>
   </si>
+  <si>
+    <t>propiedades locales y hubspot</t>
+  </si>
+  <si>
+    <t>id_location</t>
+  </si>
+  <si>
+    <t>numbre_areas</t>
+  </si>
+  <si>
+    <t>number_of_areas</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>variable local</t>
+  </si>
+  <si>
+    <t>variable Hubspot</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>id_move</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +371,14 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +388,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -379,12 +420,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -414,6 +464,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -430,10 +493,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311B0D7C-6A38-4B96-98C6-CA5BDE975B00}">
-  <dimension ref="B4:I39"/>
+  <dimension ref="B4:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,9 +1270,6 @@
       <c r="D34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="35" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
@@ -1225,9 +1281,6 @@
       <c r="D35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F35" t="s">
         <v>65</v>
       </c>
@@ -1246,9 +1299,6 @@
       <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F36" t="s">
         <v>65</v>
       </c>
@@ -1266,9 +1316,6 @@
       <c r="D37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F37" t="s">
         <v>65</v>
       </c>
@@ -1286,9 +1333,6 @@
       <c r="D38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F38" t="s">
         <v>65</v>
       </c>
@@ -1306,9 +1350,6 @@
       <c r="D39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F39" t="s">
         <v>65</v>
       </c>
@@ -1316,7 +1357,224 @@
         <v>67</v>
       </c>
     </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B59" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B44:I47"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B58:E58"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{16126FA6-1E1A-44DC-B982-852C204E70F4}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{B15EA41A-A9EA-4F22-9F3B-BA564642A0F6}"/>

</xml_diff>

<commit_message>
Se crean las asociaciones de pokemon y location en hubspot
</commit_message>
<xml_diff>
--- a/abstraccion-links.xlsx
+++ b/abstraccion-links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PokeApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2B077-4866-4D83-AE6B-EF1DDC018075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C427C03F-EE08-44B6-8DCE-F633145F7D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{134ECA9C-E322-42DE-933E-38BD1AE6EC15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="91">
   <si>
     <t>Pokémon property</t>
   </si>
@@ -317,6 +317,30 @@
   </si>
   <si>
     <t>id_move</t>
+  </si>
+  <si>
+    <t>no lo está guardando</t>
+  </si>
+  <si>
+    <t>Pokemon</t>
+  </si>
+  <si>
+    <t>id_pokemon</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>special_attack</t>
+  </si>
+  <si>
+    <t>special_defense</t>
+  </si>
+  <si>
+    <t>&lt;----- multi check</t>
+  </si>
+  <si>
+    <t>tabla</t>
   </si>
 </sst>
 </file>
@@ -388,7 +412,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -429,12 +453,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -477,6 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -812,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311B0D7C-6A38-4B96-98C6-CA5BDE975B00}">
-  <dimension ref="B4:I63"/>
+  <dimension ref="A4:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1399,7 +1433,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="15" t="s">
         <v>80</v>
       </c>
@@ -1407,7 +1441,7 @@
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
     </row>
-    <row r="50" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="12" t="s">
         <v>77</v>
       </c>
@@ -1421,7 +1455,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="11" t="s">
         <v>8</v>
       </c>
@@ -1435,7 +1469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="11" t="s">
         <v>74</v>
       </c>
@@ -1448,8 +1482,11 @@
       <c r="E52" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F52" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="11" t="s">
         <v>73</v>
       </c>
@@ -1463,7 +1500,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="11" t="s">
         <v>60</v>
       </c>
@@ -1477,7 +1514,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="11" t="s">
         <v>62</v>
       </c>
@@ -1491,7 +1528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="14" t="s">
         <v>81</v>
       </c>
@@ -1499,7 +1536,7 @@
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
     </row>
-    <row r="59" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="12" t="s">
         <v>77</v>
       </c>
@@ -1513,7 +1550,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="11" t="s">
         <v>82</v>
       </c>
@@ -1527,7 +1564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="11" t="s">
         <v>8</v>
       </c>
@@ -1541,7 +1578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="11" t="s">
         <v>52</v>
       </c>
@@ -1555,7 +1592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="11" t="s">
         <v>53</v>
       </c>
@@ -1569,11 +1606,166 @@
         <v>53</v>
       </c>
     </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B67" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>90</v>
+      </c>
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" t="s">
+        <v>86</v>
+      </c>
+      <c r="F76" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B44:I47"/>
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B66:E66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{16126FA6-1E1A-44DC-B982-852C204E70F4}"/>

</xml_diff>

<commit_message>
se arregla el id_hubspot y se guarda el que es
</commit_message>
<xml_diff>
--- a/abstraccion-links.xlsx
+++ b/abstraccion-links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PokeApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C427C03F-EE08-44B6-8DCE-F633145F7D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E694897E-293F-413B-A604-B2BB84FC0D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{134ECA9C-E322-42DE-933E-38BD1AE6EC15}"/>
+    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11235" xr2:uid="{134ECA9C-E322-42DE-933E-38BD1AE6EC15}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="92">
   <si>
     <t>Pokémon property</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>tabla</t>
+  </si>
+  <si>
+    <t>firstname</t>
   </si>
 </sst>
 </file>
@@ -501,16 +504,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311B0D7C-6A38-4B96-98C6-CA5BDE975B00}">
   <dimension ref="A4:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,46 +1395,46 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="15" t="s">
@@ -1482,7 +1485,7 @@
       <c r="E52" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="F52" s="13" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1529,12 +1532,12 @@
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="12" t="s">
@@ -1653,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>